<commit_message>
Fixed typos in the data xlsx files, changed users to don't use the prefix 'new ' on them and added a variable big enough to don't deal with rest framework pagination
</commit_message>
<xml_diff>
--- a/caluny/data/data_to_load/timetables_sheets/ing_de_la_salud.xlsx
+++ b/caluny/data/data_to_load/timetables_sheets/ing_de_la_salud.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21080" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="1º A" sheetId="1" r:id="rId1"/>
     <sheet name="2º A" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="35">
   <si>
     <t>Hora</t>
   </si>
@@ -49,9 +49,6 @@
     <t>8:45 a 10:30</t>
   </si>
   <si>
-    <t>Bioquímica Estrcutural</t>
-  </si>
-  <si>
     <t>Cálculo</t>
   </si>
   <si>
@@ -98,9 +95,6 @@
   </si>
   <si>
     <t>Ampliación de Matemáticas</t>
-  </si>
-  <si>
-    <t>Biologià Molecular y Bioquímica</t>
   </si>
   <si>
     <t>Estructuras de Datos y Algoritmos</t>
@@ -140,7 +134,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -190,6 +184,18 @@
       <sz val="8"/>
       <color rgb="FF1F497D"/>
       <name val="Verdana"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="5">
@@ -307,8 +313,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -369,7 +379,11 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -701,8 +715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -750,63 +764,63 @@
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="39">
       <c r="A4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>15</v>
-      </c>
       <c r="F4" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="39">
       <c r="A5" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>10</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>11</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="12">
       <c r="A6" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="18"/>
       <c r="C6" s="18"/>
@@ -836,7 +850,7 @@
     </row>
     <row r="8" spans="1:6" ht="12">
       <c r="A8" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
@@ -851,59 +865,59 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="D9" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="E9" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="F9" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="39">
       <c r="A10" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="D10" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="12" t="s">
-        <v>23</v>
-      </c>
       <c r="E10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="12" t="s">
         <v>19</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="39">
       <c r="A11" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="D11" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>23</v>
-      </c>
       <c r="F11" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="12">
@@ -988,6 +1002,7 @@
     <mergeCell ref="D8:F8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1000,8 +1015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1040,7 +1055,7 @@
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
       <c r="D2" s="16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
@@ -1050,64 +1065,64 @@
         <v>8</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>28</v>
-      </c>
       <c r="F3" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="39">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="E4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="39">
       <c r="A5" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="12">
       <c r="A6" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="18"/>
       <c r="C6" s="18"/>
@@ -1137,12 +1152,12 @@
     </row>
     <row r="8" spans="1:6" ht="12">
       <c r="A8" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
       <c r="D8" s="16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
@@ -1152,59 +1167,59 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="F9" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="65">
       <c r="A10" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="52">
       <c r="A11" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>35</v>
-      </c>
       <c r="F11" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="12">
@@ -1288,6 +1303,7 @@
     <mergeCell ref="D8:F8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>